<commit_message>
git ignore, assertJ, apache lang, qlearning fixes, agent new getters
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -293,43 +293,43 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="2" max="2" width="6.40625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="6.453125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="6.69140625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="6.40625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="6.69140625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="6.69140625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="6.73828125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="6.69140625" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="6.69140625" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="6.69140625" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="7.546875" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" width="7.90625" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="7.62109375" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="7.90625" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" width="7.546875" customWidth="true" bestFit="true"/>
-    <col min="17" max="17" width="7.90625" customWidth="true" bestFit="true"/>
-    <col min="18" max="18" width="7.359375" customWidth="true" bestFit="true"/>
-    <col min="19" max="19" width="7.26171875" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="7.359375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="7.26171875" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="7.359375" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="7.359375" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="7.359375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="7.359375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="7.359375" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="7.64453125" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="7.359375" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="7.62109375" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="7.26171875" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="7.546875" customWidth="true" bestFit="true"/>
-    <col min="32" max="32" width="7.359375" customWidth="true" bestFit="true"/>
-    <col min="33" max="33" width="7.71875" customWidth="true" bestFit="true"/>
-    <col min="34" max="34" width="7.359375" customWidth="true" bestFit="true"/>
-    <col min="35" max="35" width="7.62109375" customWidth="true" bestFit="true"/>
-    <col min="36" max="36" width="7.26171875" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="7.546875" customWidth="true" bestFit="true"/>
-    <col min="1" max="1" width="13.25390625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="5.83203125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="6.06640625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="6.21484375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="5.98828125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="6.21484375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="6.21484375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="6.44921875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="6.21484375" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="6.21484375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="6.21484375" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="7.10546875" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" width="7.56640625" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="7.18359375" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="7.56640625" customWidth="true" bestFit="true"/>
+    <col min="16" max="16" width="7.10546875" customWidth="true" bestFit="true"/>
+    <col min="17" max="17" width="7.56640625" customWidth="true" bestFit="true"/>
+    <col min="18" max="18" width="6.84375" customWidth="true" bestFit="true"/>
+    <col min="19" max="19" width="6.72265625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="6.84375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="6.72265625" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="6.84375" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="6.84375" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="6.84375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="6.84375" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="6.84375" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="7.2265625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="6.84375" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="7.18359375" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="6.72265625" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="7.10546875" customWidth="true" bestFit="true"/>
+    <col min="32" max="32" width="6.84375" customWidth="true" bestFit="true"/>
+    <col min="33" max="33" width="7.3046875" customWidth="true" bestFit="true"/>
+    <col min="34" max="34" width="6.84375" customWidth="true" bestFit="true"/>
+    <col min="35" max="35" width="7.18359375" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="6.72265625" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="7.10546875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="13.79296875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="45.0" customHeight="true">

</xml_diff>

<commit_message>
changed Q-value integer to double, added documentation, added BSD license information
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="40">
   <si>
     <t xml:space="preserve">X E X 
 E 0 E 
@@ -276,8 +276,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="true"/>
     </xf>
@@ -293,7 +299,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="2" max="2" width="5.83203125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="13.7421875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="6.06640625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="6.21484375" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="5.98828125" customWidth="true" bestFit="true"/>
@@ -311,7 +317,7 @@
     <col min="17" max="17" width="7.56640625" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="6.84375" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="6.72265625" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="6.84375" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="14.44921875" customWidth="true" bestFit="true"/>
     <col min="21" max="21" width="6.72265625" customWidth="true" bestFit="true"/>
     <col min="22" max="22" width="6.84375" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="6.84375" customWidth="true" bestFit="true"/>
@@ -689,7 +695,7 @@
         <v>0.0</v>
       </c>
       <c r="T4" t="n">
-        <v>0.0</v>
+        <v>-0.949999988079071</v>
       </c>
       <c r="U4" t="n">
         <v>0.0</v>
@@ -820,6 +826,988 @@
         <v>0.0</v>
       </c>
       <c r="AK5" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6" ht="45.0" customHeight="true">
+      <c r="A6"/>
+      <c r="B6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK6" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AG8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AF9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AG9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AH9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AI9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AJ9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AK9" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="n">
+        <v>3.799999952316284</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AI10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AJ10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AK10" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="11" ht="45.0" customHeight="true">
+      <c r="A11"/>
+      <c r="B11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="S11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="T11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="U11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="V11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="W11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="X11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK11" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AF12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AG12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AH12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AI12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AJ12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AK12" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AF13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AG13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AH13" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AF14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AG14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AH14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AI14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AJ14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AK14" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="n">
+        <v>3.799999952316284</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AC15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AE15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AI15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AJ15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AK15" t="n">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
improved excel printing, refactor of QLearning method, simulation management
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -6,13 +6,14 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Run #1" r:id="rId3" sheetId="1"/>
+    <sheet name="Run #0" r:id="rId3" sheetId="1"/>
+    <sheet name="Run #1" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="74">
   <si>
     <t xml:space="preserve">X E X 
 E 0 E 
@@ -230,75 +231,195 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">X E X 
+PRIZE 36 E 
+X E X 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X E X 
+E 37 E 
+X PRIZE X 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X E X 
+E 38 PRIZE 
+X E X 
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">X PRIZE X 
-B 36 E 
+E 39 E 
 X E X 
 </t>
   </si>
   <si>
     <t xml:space="preserve">X PRIZE X 
-E 37 B 
+B 40 E 
 X E X 
 </t>
   </si>
   <si>
     <t xml:space="preserve">X PRIZE X 
-E 38 E 
+E 41 B 
+X E X 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X PRIZE X 
+E 42 E 
 X B X 
 </t>
   </si>
   <si>
     <t xml:space="preserve">X B X 
-PRIZE 39 E 
-X E X 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X E X 
-PRIZE 40 B 
-X E X 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X E X 
-PRIZE 41 E 
+PRIZE 43 E 
+X E X 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X E X 
+PRIZE 44 B 
+X E X 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X E X 
+PRIZE 45 E 
 X B X 
 </t>
   </si>
   <si>
     <t xml:space="preserve">X E X 
-B 42 E 
+B 46 E 
 X PRIZE X 
 </t>
   </si>
   <si>
     <t xml:space="preserve">X B X 
-E 43 E 
+E 47 E 
 X PRIZE X 
 </t>
   </si>
   <si>
     <t xml:space="preserve">X E X 
-E 44 B 
+E 48 B 
 X PRIZE X 
 </t>
   </si>
   <si>
     <t xml:space="preserve">X E X 
-E 45 PRIZE 
+E 49 PRIZE 
 X B X 
 </t>
   </si>
   <si>
     <t xml:space="preserve">X E X 
-B 46 PRIZE 
+B 50 PRIZE 
 X E X 
 </t>
   </si>
   <si>
     <t xml:space="preserve">X B X 
-E 47 PRIZE 
-X E X 
+E 51 PRIZE 
+X E X 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X B X 
+E 52 O 
+X O X 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X B X 
+O 53 E 
+X O X 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X B X 
+O 54 O 
+X E X 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X O X 
+B 55 E 
+X O X 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X E X 
+B 56 O 
+X O X 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X O X 
+B 57 O 
+X E X 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X E X 
+O 58 O 
+X B X 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X O X 
+O 59 E 
+X B X 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X O X 
+E 60 O 
+X B X 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X E X 
+O 61 B 
+X O X 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X O X 
+O 62 B 
+X E X 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X O X 
+E 63 B 
+X O X 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X O X 
+B 64 O 
+X O X 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X O X 
+O 65 O 
+X B X 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X O X 
+O 66 B 
+X O X 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X B X 
+O 67 O 
+X O X 
 </t>
   </si>
   <si>
@@ -312,6 +433,12 @@
   </si>
   <si>
     <t>MOVE_RIGHT</t>
+  </si>
+  <si>
+    <t>Goal state achieved with -17314 points and timestep equal to 265</t>
+  </si>
+  <si>
+    <t>Goal state achieved with -17359 points and timestep equal to 295</t>
   </si>
 </sst>
 </file>
@@ -348,8 +475,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="true"/>
     </xf>
@@ -401,19 +531,39 @@
     <col min="35" max="35" width="7.18359375" customWidth="true" bestFit="true"/>
     <col min="36" max="36" width="6.72265625" customWidth="true" bestFit="true"/>
     <col min="37" max="37" width="7.10546875" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="9.75" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="10.63671875" customWidth="true" bestFit="true"/>
     <col min="39" max="39" width="9.75" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="9.75" customWidth="true" bestFit="true"/>
-    <col min="41" max="41" width="10.63671875" customWidth="true" bestFit="true"/>
-    <col min="42" max="42" width="10.76171875" customWidth="true" bestFit="true"/>
-    <col min="43" max="43" width="10.63671875" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="10.63671875" customWidth="true" bestFit="true"/>
+    <col min="41" max="41" width="9.75" customWidth="true" bestFit="true"/>
+    <col min="42" max="42" width="9.75" customWidth="true" bestFit="true"/>
+    <col min="43" max="43" width="9.75" customWidth="true" bestFit="true"/>
     <col min="44" max="44" width="9.75" customWidth="true" bestFit="true"/>
-    <col min="45" max="45" width="9.75" customWidth="true" bestFit="true"/>
-    <col min="46" max="46" width="9.75" customWidth="true" bestFit="true"/>
+    <col min="45" max="45" width="10.63671875" customWidth="true" bestFit="true"/>
+    <col min="46" max="46" width="10.76171875" customWidth="true" bestFit="true"/>
     <col min="47" max="47" width="10.63671875" customWidth="true" bestFit="true"/>
-    <col min="48" max="48" width="10.76171875" customWidth="true" bestFit="true"/>
-    <col min="49" max="49" width="10.63671875" customWidth="true" bestFit="true"/>
-    <col min="1" max="1" width="13.79296875" customWidth="true" bestFit="true"/>
+    <col min="48" max="48" width="9.75" customWidth="true" bestFit="true"/>
+    <col min="49" max="49" width="9.75" customWidth="true" bestFit="true"/>
+    <col min="50" max="50" width="9.75" customWidth="true" bestFit="true"/>
+    <col min="51" max="51" width="10.63671875" customWidth="true" bestFit="true"/>
+    <col min="52" max="52" width="10.76171875" customWidth="true" bestFit="true"/>
+    <col min="53" max="53" width="10.63671875" customWidth="true" bestFit="true"/>
+    <col min="54" max="54" width="7.10546875" customWidth="true" bestFit="true"/>
+    <col min="55" max="55" width="7.18359375" customWidth="true" bestFit="true"/>
+    <col min="56" max="56" width="7.56640625" customWidth="true" bestFit="true"/>
+    <col min="57" max="57" width="6.84375" customWidth="true" bestFit="true"/>
+    <col min="58" max="58" width="7.2265625" customWidth="true" bestFit="true"/>
+    <col min="59" max="59" width="7.2265625" customWidth="true" bestFit="true"/>
+    <col min="60" max="60" width="7.56640625" customWidth="true" bestFit="true"/>
+    <col min="61" max="61" width="7.18359375" customWidth="true" bestFit="true"/>
+    <col min="62" max="62" width="7.10546875" customWidth="true" bestFit="true"/>
+    <col min="63" max="63" width="7.3046875" customWidth="true" bestFit="true"/>
+    <col min="64" max="64" width="7.3046875" customWidth="true" bestFit="true"/>
+    <col min="65" max="65" width="6.84375" customWidth="true" bestFit="true"/>
+    <col min="66" max="66" width="7.2265625" customWidth="true" bestFit="true"/>
+    <col min="67" max="67" width="7.56640625" customWidth="true" bestFit="true"/>
+    <col min="68" max="68" width="7.3046875" customWidth="true" bestFit="true"/>
+    <col min="69" max="69" width="7.56640625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="59.79296875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="45.0" customHeight="true">
@@ -562,22 +712,82 @@
       <c r="AW1" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="AX1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="B2" t="n">
-        <v>788.0648803710938</v>
+        <v>-2.0</v>
       </c>
       <c r="C2" t="n">
         <v>0.0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0</v>
+        <v>-2.0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0</v>
+        <v>-2.0</v>
       </c>
       <c r="F2" t="n">
         <v>0.0</v>
@@ -601,7 +811,7 @@
         <v>0.0</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0</v>
+        <v>-2.0</v>
       </c>
       <c r="N2" t="n">
         <v>0.0</v>
@@ -613,22 +823,22 @@
         <v>0.0</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.0</v>
+        <v>-1000.0</v>
       </c>
       <c r="R2" t="n">
         <v>0.0</v>
       </c>
       <c r="S2" t="n">
-        <v>827.9863891601562</v>
+        <v>-2.0</v>
       </c>
       <c r="T2" t="n">
-        <v>885.3115234375</v>
+        <v>-2.0</v>
       </c>
       <c r="W2" t="n">
         <v>0.0</v>
       </c>
       <c r="Y2" t="n">
-        <v>1012.8192749023438</v>
+        <v>0.0</v>
       </c>
       <c r="Z2" t="n">
         <v>0.0</v>
@@ -637,7 +847,7 @@
         <v>0.0</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.0</v>
+        <v>-2.0</v>
       </c>
       <c r="AF2" t="n">
         <v>0.0</v>
@@ -646,7 +856,7 @@
         <v>0.0</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.0</v>
+        <v>-2.0</v>
       </c>
       <c r="AI2" t="n">
         <v>0.0</v>
@@ -661,7 +871,10 @@
         <v>0.0</v>
       </c>
       <c r="AM2" t="n">
-        <v>965.9282836914062</v>
+        <v>0.0</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>0.0</v>
       </c>
       <c r="AO2" t="n">
         <v>0.0</v>
@@ -669,11 +882,11 @@
       <c r="AP2" t="n">
         <v>0.0</v>
       </c>
-      <c r="AR2" t="n">
+      <c r="AQ2" t="n">
         <v>0.0</v>
       </c>
       <c r="AS2" t="n">
-        <v>0.0</v>
+        <v>-2.0</v>
       </c>
       <c r="AT2" t="n">
         <v>0.0</v>
@@ -682,24 +895,69 @@
         <v>0.0</v>
       </c>
       <c r="AW2" t="n">
-        <v>965.9280395507812</v>
+        <v>0.0</v>
+      </c>
+      <c r="AX2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AZ2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BA2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BB2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BC2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BD2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BE2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BF2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BG2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BK2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BL2" t="n">
+        <v>-2.0</v>
+      </c>
+      <c r="BM2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BN2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BP2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BQ2" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="B3" t="n">
-        <v>770.6630249023438</v>
+        <v>-1.0</v>
       </c>
       <c r="C3" t="n">
         <v>0.0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0</v>
+        <v>-999.0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="F3" t="n">
         <v>0.0</v>
@@ -723,7 +981,7 @@
         <v>0.0</v>
       </c>
       <c r="M3" t="n">
-        <v>0.0</v>
+        <v>-999.0</v>
       </c>
       <c r="N3" t="n">
         <v>0.0</v>
@@ -741,16 +999,16 @@
         <v>0.0</v>
       </c>
       <c r="T3" t="n">
-        <v>1011.44970703125</v>
+        <v>-1.0</v>
       </c>
       <c r="U3" t="n">
-        <v>31.201669692993164</v>
+        <v>0.0</v>
       </c>
       <c r="V3" t="n">
         <v>0.0</v>
       </c>
       <c r="X3" t="n">
-        <v>53.414146423339844</v>
+        <v>-1.0</v>
       </c>
       <c r="Z3" t="n">
         <v>0.0</v>
@@ -777,17 +1035,20 @@
         <v>0.0</v>
       </c>
       <c r="AH3" t="n">
-        <v>0.0</v>
+        <v>-999.0</v>
       </c>
       <c r="AL3" t="n">
         <v>0.0</v>
       </c>
       <c r="AM3" t="n">
-        <v>1067.17822265625</v>
+        <v>0.0</v>
       </c>
       <c r="AN3" t="n">
         <v>0.0</v>
       </c>
+      <c r="AO3" t="n">
+        <v>0.0</v>
+      </c>
       <c r="AP3" t="n">
         <v>0.0</v>
       </c>
@@ -804,24 +1065,69 @@
         <v>0.0</v>
       </c>
       <c r="AV3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AX3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AY3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AZ3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BE3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BF3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BG3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BH3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BI3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BJ3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BK3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BL3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BM3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BN3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BO3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BP3" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="B4" t="n">
-        <v>792.1668701171875</v>
+        <v>-1.0</v>
       </c>
       <c r="C4" t="n">
         <v>0.0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="F4" t="n">
         <v>0.0</v>
@@ -845,7 +1151,7 @@
         <v>0.0</v>
       </c>
       <c r="M4" t="n">
-        <v>0.0</v>
+        <v>-999.0</v>
       </c>
       <c r="N4" t="n">
         <v>0.0</v>
@@ -860,19 +1166,19 @@
         <v>0.0</v>
       </c>
       <c r="S4" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="T4" t="n">
-        <v>913.0673828125</v>
+        <v>-1.0</v>
       </c>
       <c r="U4" t="n">
-        <v>28.555679321289062</v>
+        <v>0.0</v>
       </c>
       <c r="X4" t="n">
-        <v>28.67133140563965</v>
+        <v>0.0</v>
       </c>
       <c r="Y4" t="n">
-        <v>916.6316528320312</v>
+        <v>0.0</v>
       </c>
       <c r="AC4" t="n">
         <v>0.0</v>
@@ -890,7 +1196,7 @@
         <v>0.0</v>
       </c>
       <c r="AH4" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="AI4" t="n">
         <v>0.0</v>
@@ -901,8 +1207,11 @@
       <c r="AK4" t="n">
         <v>0.0</v>
       </c>
+      <c r="AL4" t="n">
+        <v>0.0</v>
+      </c>
       <c r="AM4" t="n">
-        <v>963.9181518554688</v>
+        <v>0.0</v>
       </c>
       <c r="AN4" t="n">
         <v>0.0</v>
@@ -910,14 +1219,14 @@
       <c r="AO4" t="n">
         <v>0.0</v>
       </c>
-      <c r="AP4" t="n">
-        <v>0.0</v>
-      </c>
       <c r="AQ4" t="n">
         <v>0.0</v>
       </c>
+      <c r="AR4" t="n">
+        <v>0.0</v>
+      </c>
       <c r="AS4" t="n">
-        <v>0.0</v>
+        <v>1001.0</v>
       </c>
       <c r="AT4" t="n">
         <v>0.0</v>
@@ -926,27 +1235,1049 @@
         <v>0.0</v>
       </c>
       <c r="AW4" t="n">
-        <v>827.162841796875</v>
+        <v>0.0</v>
+      </c>
+      <c r="AX4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AY4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BA4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BB4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BC4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BD4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BH4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BI4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BJ4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BK4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BL4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BM4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BO4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BP4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BQ4" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" t="n">
+        <v>-2.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-2.0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-2.0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-1000.0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>-1000.0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>-1000.0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R5" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="S5" t="n">
+        <v>-2.0</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>-2.0</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AY5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AZ5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BA5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BB5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BC5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BD5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BE5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BF5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BG5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BH5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BI5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BJ5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BN5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BO5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BQ5" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6"/>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="2" max="2" width="5.83203125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="6.06640625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="6.21484375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="5.98828125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="6.21484375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="6.21484375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="6.44921875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="6.21484375" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="6.21484375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="6.21484375" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="7.10546875" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" width="7.56640625" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="7.18359375" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="7.56640625" customWidth="true" bestFit="true"/>
+    <col min="16" max="16" width="7.10546875" customWidth="true" bestFit="true"/>
+    <col min="17" max="17" width="7.56640625" customWidth="true" bestFit="true"/>
+    <col min="18" max="18" width="6.84375" customWidth="true" bestFit="true"/>
+    <col min="19" max="19" width="6.72265625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="6.84375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="6.72265625" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="6.84375" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="6.84375" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="6.84375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="6.84375" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="6.84375" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="7.2265625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="6.84375" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="7.18359375" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="6.72265625" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="7.10546875" customWidth="true" bestFit="true"/>
+    <col min="32" max="32" width="6.84375" customWidth="true" bestFit="true"/>
+    <col min="33" max="33" width="7.3046875" customWidth="true" bestFit="true"/>
+    <col min="34" max="34" width="6.84375" customWidth="true" bestFit="true"/>
+    <col min="35" max="35" width="7.18359375" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="6.72265625" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="7.10546875" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="10.63671875" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="9.75" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="10.63671875" customWidth="true" bestFit="true"/>
+    <col min="41" max="41" width="9.75" customWidth="true" bestFit="true"/>
+    <col min="42" max="42" width="9.75" customWidth="true" bestFit="true"/>
+    <col min="43" max="43" width="9.75" customWidth="true" bestFit="true"/>
+    <col min="44" max="44" width="9.75" customWidth="true" bestFit="true"/>
+    <col min="45" max="45" width="10.63671875" customWidth="true" bestFit="true"/>
+    <col min="46" max="46" width="10.76171875" customWidth="true" bestFit="true"/>
+    <col min="47" max="47" width="10.63671875" customWidth="true" bestFit="true"/>
+    <col min="48" max="48" width="9.75" customWidth="true" bestFit="true"/>
+    <col min="49" max="49" width="9.75" customWidth="true" bestFit="true"/>
+    <col min="50" max="50" width="9.75" customWidth="true" bestFit="true"/>
+    <col min="51" max="51" width="10.63671875" customWidth="true" bestFit="true"/>
+    <col min="52" max="52" width="10.76171875" customWidth="true" bestFit="true"/>
+    <col min="53" max="53" width="10.63671875" customWidth="true" bestFit="true"/>
+    <col min="54" max="54" width="7.10546875" customWidth="true" bestFit="true"/>
+    <col min="55" max="55" width="7.18359375" customWidth="true" bestFit="true"/>
+    <col min="56" max="56" width="7.56640625" customWidth="true" bestFit="true"/>
+    <col min="57" max="57" width="6.84375" customWidth="true" bestFit="true"/>
+    <col min="58" max="58" width="7.2265625" customWidth="true" bestFit="true"/>
+    <col min="59" max="59" width="7.2265625" customWidth="true" bestFit="true"/>
+    <col min="60" max="60" width="7.56640625" customWidth="true" bestFit="true"/>
+    <col min="61" max="61" width="7.18359375" customWidth="true" bestFit="true"/>
+    <col min="62" max="62" width="7.10546875" customWidth="true" bestFit="true"/>
+    <col min="63" max="63" width="7.3046875" customWidth="true" bestFit="true"/>
+    <col min="64" max="64" width="7.3046875" customWidth="true" bestFit="true"/>
+    <col min="65" max="65" width="6.84375" customWidth="true" bestFit="true"/>
+    <col min="66" max="66" width="7.2265625" customWidth="true" bestFit="true"/>
+    <col min="67" max="67" width="7.56640625" customWidth="true" bestFit="true"/>
+    <col min="68" max="68" width="7.3046875" customWidth="true" bestFit="true"/>
+    <col min="69" max="69" width="7.56640625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="59.79296875" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="45.0" customHeight="true">
+      <c r="A1"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AR1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AS1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AV1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AW1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AX1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AY1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AZ1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="BA1" s="2" t="s">
         <v>51</v>
       </c>
+      <c r="BB1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="BC1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="BD1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="BE1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="BF1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="BG1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="BH1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BI1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="BJ1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="BK1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="BL1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="BM1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="BN1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="BO1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="BP1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="BQ1" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="n">
+        <v>-2.0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>-2.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-2.0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-2.0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-1000.0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>-2.0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>-2.0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>-1000.0</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>-1000.0</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>-2.0</v>
+      </c>
+      <c r="T2" t="n">
+        <v>-2.0</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>-2.0</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>-2.0</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>-2.0</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AV2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AW2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AX2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AZ2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BA2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BB2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BC2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BD2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BE2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BF2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BG2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BK2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BL2" t="n">
+        <v>-2.0</v>
+      </c>
+      <c r="BM2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BN2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BP2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BQ2" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1000.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-999.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>-999.0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>-999.0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T3" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X3" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>-999.0</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>-999.0</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AU3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AV3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AX3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AY3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AZ3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BE3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BF3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BG3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BH3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BI3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BJ3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BK3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BL3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BM3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BN3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BO3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BP3" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-999.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>-999.0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>-999.0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>1000.0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AR4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>2001.0</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AW4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AX4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AY4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BA4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BB4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BC4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BD4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BH4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BI4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BJ4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BK4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BL4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BM4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BO4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BP4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BQ4" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
       <c r="B5" t="n">
-        <v>1008.440185546875</v>
+        <v>-2.0</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0</v>
+        <v>-2.0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0</v>
+        <v>-2.0</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0</v>
+        <v>-1000.0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0</v>
+        <v>-2.0</v>
       </c>
       <c r="G5" t="n">
         <v>0.0</v>
@@ -958,37 +2289,37 @@
         <v>0.0</v>
       </c>
       <c r="J5" t="n">
-        <v>0.0</v>
+        <v>-1000.0</v>
       </c>
       <c r="K5" t="n">
         <v>0.0</v>
       </c>
       <c r="L5" t="n">
-        <v>0.0</v>
+        <v>-1000.0</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0</v>
+        <v>-1000.0</v>
       </c>
       <c r="N5" t="n">
         <v>0.0</v>
       </c>
       <c r="O5" t="n">
-        <v>0.0</v>
+        <v>-1000.0</v>
       </c>
       <c r="P5" t="n">
         <v>0.0</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.0</v>
+        <v>-1000.0</v>
       </c>
       <c r="R5" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="S5" t="n">
-        <v>-109.16596984863281</v>
+        <v>-2.0</v>
       </c>
       <c r="U5" t="n">
-        <v>53.28485107421875</v>
+        <v>0.0</v>
       </c>
       <c r="V5" t="n">
         <v>0.0</v>
@@ -1003,7 +2334,7 @@
         <v>0.0</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="AC5" t="n">
         <v>0.0</v>
@@ -1026,20 +2357,23 @@
       <c r="AL5" t="n">
         <v>0.0</v>
       </c>
+      <c r="AM5" t="n">
+        <v>0.0</v>
+      </c>
       <c r="AN5" t="n">
         <v>0.0</v>
       </c>
       <c r="AO5" t="n">
         <v>0.0</v>
       </c>
-      <c r="AQ5" t="n">
+      <c r="AP5" t="n">
         <v>0.0</v>
       </c>
       <c r="AR5" t="n">
         <v>0.0</v>
       </c>
       <c r="AS5" t="n">
-        <v>0.0</v>
+        <v>-2.0</v>
       </c>
       <c r="AU5" t="n">
         <v>0.0</v>
@@ -1048,7 +2382,58 @@
         <v>0.0</v>
       </c>
       <c r="AW5" t="n">
-        <v>767.048583984375</v>
+        <v>0.0</v>
+      </c>
+      <c r="AY5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AZ5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BA5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BB5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BC5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BD5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BE5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BF5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BG5" t="n">
+        <v>-999.0</v>
+      </c>
+      <c r="BH5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BI5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BJ5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BN5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BO5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BQ5" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6"/>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>